<commit_message>
Added lipids adduct relation rules
</commit_message>
<xml_diff>
--- a/src/main/resources/ceu/biolab/cmm/scoreAnnotations/model/ScoreLipidsRules.drl.xlsx
+++ b/src/main/resources/ceu/biolab/cmm/scoreAnnotations/model/ScoreLipidsRules.drl.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="60">
   <si>
     <t xml:space="preserve">RuleSet</t>
   </si>
@@ -107,6 +107,99 @@
   </si>
   <si>
     <t xml:space="preserve">(int)$compB.getNumberCarbons(),(int)$compA.getNumberCarbons()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RuleTable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adduct Relation Rule Table for Lipids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$compA: EvaluatedLipid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$compB: EvaluatedLipid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$compC: EvaluatedLipid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getAdduct()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getFeatureRtValue() &gt; $1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getCompoundId() != $1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getCompoundId() == $1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Math.abs(getFeatureRtValue() - $1) &lt; 0.05d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getFeatureRtValue() == $1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$compA.setAdductRelationScore($1);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$compA.setIonizationScore($1);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adduct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M+Na</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M+H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$compA.getCompoundId()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$compA.getFeatureRtValue()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M+K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B7</t>
   </si>
 </sst>
 </file>
@@ -199,7 +292,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -217,6 +310,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -403,23 +500,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:N91"/>
   <sheetViews>
     <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13:B14"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="22.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="64.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="66.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="11" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="24.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="37.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="34.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="14" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,10 +746,614 @@
         <v>25</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" s="1"/>
+      <c r="L19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="L20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="L21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="L22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J74" s="1"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J76" s="1"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J77" s="1"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J78" s="1"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J79" s="1"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J80" s="1"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J81" s="1"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J82" s="1"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J83" s="1"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J84" s="1"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J85" s="1"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J86" s="1"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J87" s="1"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J88" s="1"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J89" s="1"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J90" s="1"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J91" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:H6"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>